<commit_message>
add some file 2017-1-17
</commit_message>
<xml_diff>
--- a/Data/全部数据/原始excel/理想数据k=1~2/k=1.0/k=1.0所有概率值.xlsx
+++ b/Data/全部数据/原始excel/理想数据k=1~2/k=1.0/k=1.0所有概率值.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="10470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>LZ-调节2hz_20160601_110006_ASIC_EEG</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>wzq-调节2Hz_20161214_103206_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>wnb-调节6Hz_20161230_113123_ASIC_EEG</t>
+  </si>
+  <si>
+    <t>wnb-调节6Hz_20170110_113300_ASIC_EEG</t>
   </si>
 </sst>
 </file>
@@ -437,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AB3"/>
+      <selection sqref="A1:AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,8 +536,14 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.59039548022598876</v>
       </c>
@@ -616,8 +628,14 @@
       <c r="AB2">
         <v>0.53745928338762217</v>
       </c>
+      <c r="AC2">
+        <v>0.59485530546623799</v>
+      </c>
+      <c r="AD2">
+        <v>0.49838187702265369</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.68100358422939067</v>
       </c>
@@ -701,6 +719,12 @@
       </c>
       <c r="AB3">
         <v>0.54019292604501601</v>
+      </c>
+      <c r="AC3">
+        <v>0.56211180124223603</v>
+      </c>
+      <c r="AD3">
+        <v>0.70648464163822533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>